<commit_message>
Added two user stories based off of what we were coming up with in class.
</commit_message>
<xml_diff>
--- a/documentation/Product Backlog.xlsx
+++ b/documentation/Product Backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20405"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeffr\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\demmons1\UWG-SE2-Group5-Myst\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6536B05-F926-41B5-AA65-88EEEC846D1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFBE24E0-B209-4AB1-A8F4-FB79E0CC7C5C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,12 +45,6 @@
     <t>I want to…</t>
   </si>
   <si>
-    <t>enter resources</t>
-  </si>
-  <si>
-    <t>overview budget</t>
-  </si>
-  <si>
     <t>setup build stages</t>
   </si>
   <si>
@@ -72,9 +66,6 @@
     <t>share calendar with constructor</t>
   </si>
   <si>
-    <t>I can review the overall budget for the project</t>
-  </si>
-  <si>
     <t>I can track the steps needed to complete the project</t>
   </si>
   <si>
@@ -87,9 +78,6 @@
     <t>I can update how resources are/have been used during the process</t>
   </si>
   <si>
-    <t>I can track the costs (materials and contractors) needed to complete the project</t>
-  </si>
-  <si>
     <t>I can review the resources (materials and contractors) needed to complete the project</t>
   </si>
   <si>
@@ -100,6 +88,18 @@
   </si>
   <si>
     <t>I can share the timeline for the project with contractors to ensure everyone is aware of when steps need to be completed and what steps have already been completed</t>
+  </si>
+  <si>
+    <t>Add games that I own/enjoy</t>
+  </si>
+  <si>
+    <t>I can keep track of all the games in my collection</t>
+  </si>
+  <si>
+    <t>Communicate with others with the same game</t>
+  </si>
+  <si>
+    <t>I can find new friends/ get and share (port) information about the game</t>
   </si>
 </sst>
 </file>
@@ -427,17 +427,17 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="37.5703125" customWidth="1"/>
-    <col min="4" max="4" width="153.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.59765625" customWidth="1"/>
+    <col min="3" max="3" width="37.59765625" customWidth="1"/>
+    <col min="4" max="4" width="153.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -451,7 +451,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -459,13 +459,13 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
@@ -473,13 +473,13 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>1</v>
       </c>
@@ -487,13 +487,13 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>1</v>
       </c>
@@ -501,13 +501,13 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>2</v>
       </c>
@@ -518,10 +518,10 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>2</v>
       </c>
@@ -529,13 +529,13 @@
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>2</v>
       </c>
@@ -543,13 +543,13 @@
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>3</v>
       </c>
@@ -557,13 +557,13 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>4</v>
       </c>
@@ -571,13 +571,13 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>5</v>
       </c>
@@ -585,14 +585,14 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D8">
+  <sortState ref="A2:D8">
     <sortCondition ref="A2:A8"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added directory for Use Case Scenarios
</commit_message>
<xml_diff>
--- a/documentation/Product Backlog.xlsx
+++ b/documentation/Product Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20405"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\demmons1\UWG-SE2-Group5-Myst\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/de0b3ea1232571d3/Documents/School/Spring 24/SE2/SE2-Group5-Myst/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFBE24E0-B209-4AB1-A8F4-FB79E0CC7C5C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{EFBE24E0-B209-4AB1-A8F4-FB79E0CC7C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B511A676-D6E8-43BB-906F-25397598FA0F}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2640" yWindow="2640" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Priority</t>
   </si>
@@ -39,60 +39,9 @@
     <t>User</t>
   </si>
   <si>
-    <t>attach resources to build stage</t>
-  </si>
-  <si>
     <t>I want to…</t>
   </si>
   <si>
-    <t>setup build stages</t>
-  </si>
-  <si>
-    <t>overview build process</t>
-  </si>
-  <si>
-    <t>reassign resources</t>
-  </si>
-  <si>
-    <t>overview resources</t>
-  </si>
-  <si>
-    <t>attach inspection to build stage</t>
-  </si>
-  <si>
-    <t>add prerequisites to build stage</t>
-  </si>
-  <si>
-    <t>share calendar with constructor</t>
-  </si>
-  <si>
-    <t>I can track the steps needed to complete the project</t>
-  </si>
-  <si>
-    <t>I can review the steps needed to compelte the project</t>
-  </si>
-  <si>
-    <t>I can track resources needed for specific steps of the process</t>
-  </si>
-  <si>
-    <t>I can update how resources are/have been used during the process</t>
-  </si>
-  <si>
-    <t>I can review the resources (materials and contractors) needed to complete the project</t>
-  </si>
-  <si>
-    <t>I can indicate an inspection  need to be complete after the other work for a particular step of the process</t>
-  </si>
-  <si>
-    <t>I can indicate other steps that must be completed before beginning a step of the process</t>
-  </si>
-  <si>
-    <t>I can share the timeline for the project with contractors to ensure everyone is aware of when steps need to be completed and what steps have already been completed</t>
-  </si>
-  <si>
-    <t>Add games that I own/enjoy</t>
-  </si>
-  <si>
     <t>I can keep track of all the games in my collection</t>
   </si>
   <si>
@@ -100,6 +49,9 @@
   </si>
   <si>
     <t>I can find new friends/ get and share (port) information about the game</t>
+  </si>
+  <si>
+    <t>Select games that I own/enjoy</t>
   </si>
 </sst>
 </file>
@@ -424,20 +376,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.59765625" customWidth="1"/>
-    <col min="3" max="3" width="37.59765625" customWidth="1"/>
-    <col min="4" max="4" width="153.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="37.5703125" customWidth="1"/>
+    <col min="4" max="4" width="153.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -445,13 +397,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -459,13 +411,13 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -473,126 +425,19 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A4">
-        <v>1</v>
-      </c>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A9">
-        <v>3</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A10">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A11">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" t="s">
-        <v>20</v>
-      </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D8">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D8">
     <sortCondition ref="A2:A8"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>